<commit_message>
mkdir backend and celery
</commit_message>
<xml_diff>
--- a/my_progress.xlsx
+++ b/my_progress.xlsx
@@ -413,13 +413,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -439,6 +445,50 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>Похудение</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Стартовый вес, кг</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Текущий вес, кг</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Цель, кг</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Прогресс, %</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>90.0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>50.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>20.0</t>
         </is>
       </c>
     </row>

</xml_diff>